<commit_message>
save increase/decrease calc in excel
</commit_message>
<xml_diff>
--- a/data_experiments/ArcA_nch_new.xlsx
+++ b/data_experiments/ArcA_nch_new.xlsx
@@ -1,15 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Floodlight\ft_Regulation_Katrin\data_experiments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A27F354-2470-47AC-A86B-7F7832162D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -331,8 +348,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,15 +408,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,7 +466,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -473,9 +498,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,6 +550,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,14 +743,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,7 +775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -723,22 +786,30 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>1.017</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="E2">
-        <v>1.017</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="F2">
-        <v>7.477381962160287</v>
+        <v>7.4773819621602868</v>
       </c>
       <c r="G2">
-        <v>7.352391309892122</v>
+        <v>7.3523913098921216</v>
       </c>
       <c r="H2">
-        <v>7.477381962160287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>7.4773819621602868</v>
+      </c>
+      <c r="K2">
+        <f>E2/D2</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>H2/F2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -749,10 +820,10 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>1.611090358074832</v>
+        <v>1.6110903580748319</v>
       </c>
       <c r="E3">
-        <v>2.61847082097539</v>
+        <v>2.6184708209753902</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -763,8 +834,16 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="K3">
+        <f>E3/D3</f>
+        <v>1.6252786864818214</v>
+      </c>
+      <c r="L3" t="e">
+        <f>H3/F3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -775,22 +854,30 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0.789</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="E4">
-        <v>0.789</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="F4">
         <v>4.860861146496827</v>
       </c>
       <c r="G4">
-        <v>6.160787257917398</v>
+        <v>6.1607872579173977</v>
       </c>
       <c r="H4">
         <v>4.860861146496827</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="K4">
+        <f>E4/D4</f>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f>H4/F4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -807,16 +894,24 @@
         <v>3.75</v>
       </c>
       <c r="F5">
-        <v>-16.02352614316763</v>
+        <v>-16.023526143167629</v>
       </c>
       <c r="G5">
-        <v>-4.272940304844702</v>
+        <v>-4.2729403048447017</v>
       </c>
       <c r="H5">
-        <v>-16.02352614316763</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-16.023526143167629</v>
+      </c>
+      <c r="K5">
+        <f>E5/D5</f>
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f>H5/F5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -827,22 +922,30 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>1.656</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="E6">
-        <v>1.656</v>
+        <v>1.6559999999999999</v>
       </c>
       <c r="F6">
-        <v>4.959984944574645</v>
+        <v>4.9599849445746447</v>
       </c>
       <c r="G6">
-        <v>2.995159990685172</v>
+        <v>2.9951599906851718</v>
       </c>
       <c r="H6">
-        <v>4.959984944574645</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>4.9599849445746447</v>
+      </c>
+      <c r="K6">
+        <f>E6/D6</f>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f>H6/F6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -867,8 +970,16 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="K7">
+        <f>E7/D7</f>
+        <v>1</v>
+      </c>
+      <c r="L7" t="e">
+        <f>H7/F7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -893,8 +1004,16 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="K8">
+        <f>E8/D8</f>
+        <v>1</v>
+      </c>
+      <c r="L8" t="e">
+        <f>H8/F8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -911,16 +1030,24 @@
         <v>1.371</v>
       </c>
       <c r="F9">
-        <v>-14.71613956874286</v>
+        <v>-14.716139568742861</v>
       </c>
       <c r="G9">
         <v>-10.73387277078254</v>
       </c>
       <c r="H9">
-        <v>-14.71613956874286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>-14.716139568742861</v>
+      </c>
+      <c r="K9">
+        <f>E9/D9</f>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>H9/F9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -937,16 +1064,24 @@
         <v>1.653</v>
       </c>
       <c r="F10">
-        <v>3.214895047684765</v>
+        <v>3.2148950476847649</v>
       </c>
       <c r="G10">
         <v>1.944885086318672</v>
       </c>
       <c r="H10">
-        <v>3.214895047684765</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>3.2148950476847649</v>
+      </c>
+      <c r="K10">
+        <f>E10/D10</f>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f>H10/F10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -957,10 +1092,10 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="E11">
-        <v>2.22</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -971,8 +1106,16 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="K11">
+        <f>E11/D11</f>
+        <v>1</v>
+      </c>
+      <c r="L11" t="e">
+        <f>H11/F11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -997,8 +1140,16 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="K12">
+        <f>E12/D12</f>
+        <v>1</v>
+      </c>
+      <c r="L12" t="e">
+        <f>H12/F12</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1012,7 +1163,7 @@
         <v>1.280927334201551</v>
       </c>
       <c r="E13">
-        <v>2.232700086700888</v>
+        <v>2.2327000867008882</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1023,8 +1174,16 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="K13">
+        <f>E13/D13</f>
+        <v>1.7430341496245858</v>
+      </c>
+      <c r="L13" t="e">
+        <f>H13/F13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1035,22 +1194,30 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>0.912</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="E14">
-        <v>0.912</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="F14">
         <v>2.504309470368745</v>
       </c>
       <c r="G14">
-        <v>2.745953366632396</v>
+        <v>2.7459533666323961</v>
       </c>
       <c r="H14">
         <v>2.504309470368745</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="K14">
+        <f>E14/D14</f>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>H14/F14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1061,22 +1228,30 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>1.142</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="E15">
-        <v>0.2408000264888858</v>
+        <v>0.24080002648888579</v>
       </c>
       <c r="F15">
-        <v>6.007249575350351</v>
+        <v>6.0072495753503512</v>
       </c>
       <c r="G15">
-        <v>5.260288594877716</v>
+        <v>5.2602885948777161</v>
       </c>
       <c r="H15">
-        <v>1.266677632985738</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>1.2666776329857381</v>
+      </c>
+      <c r="K15">
+        <f>E15/D15</f>
+        <v>0.21085816680287725</v>
+      </c>
+      <c r="L15">
+        <f>H15/F15</f>
+        <v>0.21085816680287728</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1087,22 +1262,30 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>1.263</v>
+        <v>1.2629999999999999</v>
       </c>
       <c r="E16">
         <v>0.3168530504375211</v>
       </c>
       <c r="F16">
-        <v>6.007249575350358</v>
+        <v>6.0072495753503583</v>
       </c>
       <c r="G16">
-        <v>4.756333788875977</v>
+        <v>4.7563337888759767</v>
       </c>
       <c r="H16">
-        <v>1.507058869904406</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>1.5070588699044061</v>
+      </c>
+      <c r="K16">
+        <f>E16/D16</f>
+        <v>0.25087335743271666</v>
+      </c>
+      <c r="L16">
+        <f>H16/F16</f>
+        <v>0.25087335743271671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1113,22 +1296,30 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>2.061</v>
+        <v>2.0609999999999999</v>
       </c>
       <c r="E17">
-        <v>2.061</v>
+        <v>2.0609999999999999</v>
       </c>
       <c r="F17">
-        <v>8.390000000000001</v>
+        <v>8.39</v>
       </c>
       <c r="G17">
-        <v>4.070839398350316</v>
+        <v>4.0708393983503157</v>
       </c>
       <c r="H17">
-        <v>8.390000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>8.39</v>
+      </c>
+      <c r="K17">
+        <f>E17/D17</f>
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f>H17/F17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1153,8 +1344,16 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="K18">
+        <f>E18/D18</f>
+        <v>1</v>
+      </c>
+      <c r="L18" t="e">
+        <f>H18/F18</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1179,8 +1378,16 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="K19">
+        <f>E19/D19</f>
+        <v>1</v>
+      </c>
+      <c r="L19" t="e">
+        <f>H19/F19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1191,10 +1398,10 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <v>0.734</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="E20">
-        <v>0.734</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1205,8 +1412,16 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="K20">
+        <f>E20/D20</f>
+        <v>1</v>
+      </c>
+      <c r="L20" t="e">
+        <f>H20/F20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1217,10 +1432,10 @@
         <v>26</v>
       </c>
       <c r="D21">
-        <v>1.201</v>
+        <v>1.2010000000000001</v>
       </c>
       <c r="E21">
-        <v>1.201</v>
+        <v>1.2010000000000001</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1231,8 +1446,16 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="K21">
+        <f>E21/D21</f>
+        <v>1</v>
+      </c>
+      <c r="L21" t="e">
+        <f>H21/F21</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1246,19 +1469,27 @@
         <v>1.129</v>
       </c>
       <c r="E22">
-        <v>0.2333461904893545</v>
+        <v>0.23334619048935451</v>
       </c>
       <c r="F22">
-        <v>5.064375661482109</v>
+        <v>5.0643756614821092</v>
       </c>
       <c r="G22">
-        <v>4.485718034970867</v>
+        <v>4.4857180349708674</v>
       </c>
       <c r="H22">
-        <v>1.046725215069845</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>1.0467252150698449</v>
+      </c>
+      <c r="K22">
+        <f>E22/D22</f>
+        <v>0.20668395968941941</v>
+      </c>
+      <c r="L22">
+        <f>H22/F22</f>
+        <v>0.20668395968941941</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1269,22 +1500,30 @@
         <v>28</v>
       </c>
       <c r="D23">
-        <v>3.167</v>
+        <v>3.1669999999999998</v>
       </c>
       <c r="E23">
-        <v>3.167</v>
+        <v>3.1669999999999998</v>
       </c>
       <c r="F23">
-        <v>45.51400977451759</v>
+        <v>45.514009774517589</v>
       </c>
       <c r="G23">
-        <v>14.37133242011923</v>
+        <v>14.371332420119231</v>
       </c>
       <c r="H23">
-        <v>45.51400977451759</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>45.514009774517589</v>
+      </c>
+      <c r="K23">
+        <f>E23/D23</f>
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f>H23/F23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1309,8 +1548,16 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="K24">
+        <f>E24/D24</f>
+        <v>1</v>
+      </c>
+      <c r="L24" t="e">
+        <f>H24/F24</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1321,10 +1568,10 @@
         <v>30</v>
       </c>
       <c r="D25">
-        <v>1.685</v>
+        <v>1.6850000000000001</v>
       </c>
       <c r="E25">
-        <v>1.685</v>
+        <v>1.6850000000000001</v>
       </c>
       <c r="F25">
         <v>1.758177444106805</v>
@@ -1335,8 +1582,16 @@
       <c r="H25">
         <v>1.758177444106805</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="K25">
+        <f>E25/D25</f>
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <f>H25/F25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1356,13 +1611,21 @@
         <v>0.8739215069684303</v>
       </c>
       <c r="G26">
-        <v>0.5945044265091363</v>
+        <v>0.59450442650913626</v>
       </c>
       <c r="H26">
         <v>0.8739215069684303</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="K26">
+        <f>E26/D26</f>
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f>H26/F26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1373,10 +1636,10 @@
         <v>32</v>
       </c>
       <c r="D27">
-        <v>2.479</v>
+        <v>2.4790000000000001</v>
       </c>
       <c r="E27">
-        <v>2.479</v>
+        <v>2.4790000000000001</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1387,8 +1650,16 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="K27">
+        <f>E27/D27</f>
+        <v>1</v>
+      </c>
+      <c r="L27" t="e">
+        <f>H27/F27</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1405,16 +1676,24 @@
         <v>1.65</v>
       </c>
       <c r="F28">
-        <v>-22.809833310205</v>
+        <v>-22.809833310205001</v>
       </c>
       <c r="G28">
         <v>-13.82414140012424</v>
       </c>
       <c r="H28">
-        <v>-22.809833310205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>-22.809833310205001</v>
+      </c>
+      <c r="K28">
+        <f>E28/D28</f>
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f>H28/F28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1425,22 +1704,30 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>3.422</v>
+        <v>3.4220000000000002</v>
       </c>
       <c r="E29">
-        <v>3.422</v>
+        <v>3.4220000000000002</v>
       </c>
       <c r="F29">
         <v>2.678481850507521</v>
       </c>
       <c r="G29">
-        <v>0.7827240942453305</v>
+        <v>0.78272409424533052</v>
       </c>
       <c r="H29">
         <v>2.678481850507521</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="K29">
+        <f>E29/D29</f>
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <f>H29/F29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1451,22 +1738,30 @@
         <v>35</v>
       </c>
       <c r="D30">
-        <v>1.021</v>
+        <v>1.0209999999999999</v>
       </c>
       <c r="E30">
-        <v>0.1767033788738809</v>
+        <v>0.17670337887388091</v>
       </c>
       <c r="F30">
-        <v>6.007249575350351</v>
+        <v>6.0072495753503512</v>
       </c>
       <c r="G30">
-        <v>5.883692042458718</v>
+        <v>5.8836920424587182</v>
       </c>
       <c r="H30">
         <v>1.039668264155821</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="K30">
+        <f>E30/D30</f>
+        <v>0.17306893131623988</v>
+      </c>
+      <c r="L30">
+        <f>H30/F30</f>
+        <v>0.17306893131623988</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1477,22 +1772,30 @@
         <v>36</v>
       </c>
       <c r="D31">
-        <v>1.499</v>
+        <v>1.4990000000000001</v>
       </c>
       <c r="E31">
-        <v>1.499</v>
+        <v>1.4990000000000001</v>
       </c>
       <c r="F31">
-        <v>-2.281503094067124</v>
+        <v>-2.2815030940671241</v>
       </c>
       <c r="G31">
         <v>-1.522016740538441</v>
       </c>
       <c r="H31">
-        <v>-2.281503094067124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>-2.2815030940671241</v>
+      </c>
+      <c r="K31">
+        <f>E31/D31</f>
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <f>H31/F31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1506,7 +1809,7 @@
         <v>1.95</v>
       </c>
       <c r="E32">
-        <v>0.9776720462805529</v>
+        <v>0.97767204628055293</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1517,8 +1820,16 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="K32">
+        <f>E32/D32</f>
+        <v>0.5013702801438733</v>
+      </c>
+      <c r="L32" t="e">
+        <f>H32/F32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1532,19 +1843,27 @@
         <v>1.274649847289983</v>
       </c>
       <c r="E33">
-        <v>2.224483160761743</v>
+        <v>2.2244831607617428</v>
       </c>
       <c r="F33">
         <v>43.59898531199763</v>
       </c>
       <c r="G33">
-        <v>34.20467621338744</v>
+        <v>34.204676213387437</v>
       </c>
       <c r="H33">
-        <v>76.0877262559881</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>76.087726255988102</v>
+      </c>
+      <c r="K33">
+        <f>E33/D33</f>
+        <v>1.7451719509410277</v>
+      </c>
+      <c r="L33">
+        <f>H33/F33</f>
+        <v>1.7451719509410273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1555,7 +1874,7 @@
         <v>39</v>
       </c>
       <c r="D34">
-        <v>2.509</v>
+        <v>2.5089999999999999</v>
       </c>
       <c r="E34">
         <v>1.774132758433931</v>
@@ -1569,8 +1888,16 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="K34">
+        <f>E34/D34</f>
+        <v>0.70710751631483904</v>
+      </c>
+      <c r="L34" t="e">
+        <f>H34/F34</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1581,22 +1908,30 @@
         <v>40</v>
       </c>
       <c r="D35">
-        <v>1.932</v>
+        <v>1.9319999999999999</v>
       </c>
       <c r="E35">
-        <v>1.932</v>
+        <v>1.9319999999999999</v>
       </c>
       <c r="F35">
-        <v>14.71613956874286</v>
+        <v>14.716139568742861</v>
       </c>
       <c r="G35">
-        <v>7.617049466223014</v>
+        <v>7.6170494662230137</v>
       </c>
       <c r="H35">
-        <v>14.71613956874286</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>14.716139568742861</v>
+      </c>
+      <c r="K35">
+        <f>E35/D35</f>
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <f>H35/F35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1621,8 +1956,16 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="K36">
+        <f>E36/D36</f>
+        <v>1</v>
+      </c>
+      <c r="L36" t="e">
+        <f>H36/F36</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1647,8 +1990,16 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="K37">
+        <f>E37/D37</f>
+        <v>1</v>
+      </c>
+      <c r="L37" t="e">
+        <f>H37/F37</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1662,19 +2013,27 @@
         <v>1.629</v>
       </c>
       <c r="E38">
-        <v>0.6211868155320407</v>
+        <v>0.62118681553204069</v>
       </c>
       <c r="F38">
-        <v>5.064375661482109</v>
+        <v>5.0643756614821092</v>
       </c>
       <c r="G38">
-        <v>3.108886225587544</v>
+        <v>3.1088862255875438</v>
       </c>
       <c r="H38">
-        <v>1.931199134324152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>1.9311991343241519</v>
+      </c>
+      <c r="K38">
+        <f>E38/D38</f>
+        <v>0.38133015072562348</v>
+      </c>
+      <c r="L38">
+        <f>H38/F38</f>
+        <v>0.38133015072562348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1688,19 +2047,27 @@
         <v>3.3</v>
       </c>
       <c r="E39">
-        <v>3.186063301937858</v>
+        <v>3.1860633019378581</v>
       </c>
       <c r="F39">
-        <v>-5.064375661482109</v>
+        <v>-5.0643756614821092</v>
       </c>
       <c r="G39">
-        <v>-1.534659291358215</v>
+        <v>-1.5346592913582151</v>
       </c>
       <c r="H39">
-        <v>-4.889521649174368</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>-4.8895216491743678</v>
+      </c>
+      <c r="K39">
+        <f>E39/D39</f>
+        <v>0.96547372785995711</v>
+      </c>
+      <c r="L39">
+        <f>H39/F39</f>
+        <v>0.965473727859957</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1717,16 +2084,24 @@
         <v>2.996</v>
       </c>
       <c r="F40">
-        <v>1.496983757261562</v>
+        <v>1.4969837572615621</v>
       </c>
       <c r="G40">
-        <v>0.4996608001540594</v>
+        <v>0.49966080015405939</v>
       </c>
       <c r="H40">
-        <v>1.496983757261562</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>1.4969837572615621</v>
+      </c>
+      <c r="K40">
+        <f>E40/D40</f>
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <f>H40/F40</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1737,10 +2112,10 @@
         <v>46</v>
       </c>
       <c r="D41">
-        <v>2.619</v>
+        <v>2.6190000000000002</v>
       </c>
       <c r="E41">
-        <v>2.619</v>
+        <v>2.6190000000000002</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1751,8 +2126,16 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="K41">
+        <f>E41/D41</f>
+        <v>1</v>
+      </c>
+      <c r="L41" t="e">
+        <f>H41/F41</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1763,22 +2146,30 @@
         <v>47</v>
       </c>
       <c r="D42">
-        <v>1.058</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="E42">
-        <v>1.058</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="F42">
-        <v>1.496983757261562</v>
+        <v>1.4969837572615621</v>
       </c>
       <c r="G42">
-        <v>1.41491848512435</v>
+        <v>1.4149184851243499</v>
       </c>
       <c r="H42">
-        <v>1.496983757261562</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>1.4969837572615621</v>
+      </c>
+      <c r="K42">
+        <f>E42/D42</f>
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <f>H42/F42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1795,16 +2186,24 @@
         <v>1.744</v>
       </c>
       <c r="F43">
-        <v>1.181498093245959</v>
+        <v>1.1814980932459589</v>
       </c>
       <c r="G43">
-        <v>0.677464503008004</v>
+        <v>0.67746450300800398</v>
       </c>
       <c r="H43">
-        <v>1.181498093245959</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>1.1814980932459589</v>
+      </c>
+      <c r="K43">
+        <f>E43/D43</f>
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <f>H43/F43</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1815,22 +2214,30 @@
         <v>49</v>
       </c>
       <c r="D44">
-        <v>0.676</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="E44">
-        <v>0.676</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F44">
-        <v>7.477381962160287</v>
+        <v>7.4773819621602868</v>
       </c>
       <c r="G44">
-        <v>11.06121592035545</v>
+        <v>11.061215920355449</v>
       </c>
       <c r="H44">
-        <v>7.477381962160287</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>7.4773819621602868</v>
+      </c>
+      <c r="K44">
+        <f>E44/D44</f>
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <f>H44/F44</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1855,8 +2262,16 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="K45">
+        <f>E45/D45</f>
+        <v>1</v>
+      </c>
+      <c r="L45" t="e">
+        <f>H45/F45</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1881,8 +2296,16 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="K46">
+        <f>E46/D46</f>
+        <v>1</v>
+      </c>
+      <c r="L46" t="e">
+        <f>H46/F46</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1907,8 +2330,16 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="K47">
+        <f>E47/D47</f>
+        <v>1</v>
+      </c>
+      <c r="L47" t="e">
+        <f>H47/F47</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1919,22 +2350,30 @@
         <v>53</v>
       </c>
       <c r="D48">
-        <v>1.447</v>
+        <v>1.4470000000000001</v>
       </c>
       <c r="E48">
-        <v>1.447</v>
+        <v>1.4470000000000001</v>
       </c>
       <c r="F48">
-        <v>22.809833310205</v>
+        <v>22.809833310205001</v>
       </c>
       <c r="G48">
         <v>15.76353373200069</v>
       </c>
       <c r="H48">
-        <v>22.809833310205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>22.809833310205001</v>
+      </c>
+      <c r="K48">
+        <f>E48/D48</f>
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <f>H48/F48</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1959,8 +2398,16 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="K49">
+        <f>E49/D49</f>
+        <v>1</v>
+      </c>
+      <c r="L49" t="e">
+        <f>H49/F49</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1985,8 +2432,16 @@
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="K50">
+        <f>E50/D50</f>
+        <v>1</v>
+      </c>
+      <c r="L50" t="e">
+        <f>H50/F50</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2011,8 +2466,16 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="K51">
+        <f>E51/D51</f>
+        <v>1</v>
+      </c>
+      <c r="L51" t="e">
+        <f>H51/F51</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2023,10 +2486,10 @@
         <v>57</v>
       </c>
       <c r="D52">
-        <v>1.551</v>
+        <v>1.5509999999999999</v>
       </c>
       <c r="E52">
-        <v>1.551</v>
+        <v>1.5509999999999999</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2037,8 +2500,16 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="K52">
+        <f>E52/D52</f>
+        <v>1</v>
+      </c>
+      <c r="L52" t="e">
+        <f>H52/F52</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2049,22 +2520,30 @@
         <v>58</v>
       </c>
       <c r="D53">
-        <v>2.064</v>
+        <v>2.0640000000000001</v>
       </c>
       <c r="E53">
-        <v>2.064</v>
+        <v>2.0640000000000001</v>
       </c>
       <c r="F53">
         <v>-10</v>
       </c>
       <c r="G53">
-        <v>-4.844961240310077</v>
+        <v>-4.8449612403100772</v>
       </c>
       <c r="H53">
         <v>-10</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="K53">
+        <f>E53/D53</f>
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <f>H53/F53</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2089,8 +2568,16 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="K54">
+        <f>E54/D54</f>
+        <v>1</v>
+      </c>
+      <c r="L54" t="e">
+        <f>H54/F54</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2101,10 +2588,10 @@
         <v>60</v>
       </c>
       <c r="D55">
-        <v>2.493</v>
+        <v>2.4929999999999999</v>
       </c>
       <c r="E55">
-        <v>2.493</v>
+        <v>2.4929999999999999</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2115,8 +2602,16 @@
       <c r="H55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="K55">
+        <f>E55/D55</f>
+        <v>1</v>
+      </c>
+      <c r="L55" t="e">
+        <f>H55/F55</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2133,16 +2628,24 @@
         <v>1.246</v>
       </c>
       <c r="F56">
-        <v>17.53086542978666</v>
+        <v>17.530865429786662</v>
       </c>
       <c r="G56">
         <v>14.06971543321562</v>
       </c>
       <c r="H56">
-        <v>17.53086542978666</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>17.530865429786662</v>
+      </c>
+      <c r="K56">
+        <f>E56/D56</f>
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <f>H56/F56</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2167,8 +2670,16 @@
       <c r="H57">
         <v>29.1758271355658</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="K57">
+        <f>E57/D57</f>
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <f>H57/F57</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2193,8 +2704,16 @@
       <c r="H58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="K58">
+        <f>E58/D58</f>
+        <v>1</v>
+      </c>
+      <c r="L58" t="e">
+        <f>H58/F58</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2205,10 +2724,10 @@
         <v>64</v>
       </c>
       <c r="D59">
-        <v>2.844</v>
+        <v>2.8439999999999999</v>
       </c>
       <c r="E59">
-        <v>2.844</v>
+        <v>2.8439999999999999</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2219,8 +2738,16 @@
       <c r="H59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="K59">
+        <f>E59/D59</f>
+        <v>1</v>
+      </c>
+      <c r="L59" t="e">
+        <f>H59/F59</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2237,16 +2764,24 @@
         <v>1.591</v>
       </c>
       <c r="F60">
-        <v>-4.765319193197463</v>
+        <v>-4.7653191931974632</v>
       </c>
       <c r="G60">
-        <v>-2.995172340161825</v>
+        <v>-2.9951723401618251</v>
       </c>
       <c r="H60">
-        <v>-4.765319193197463</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>-4.7653191931974632</v>
+      </c>
+      <c r="K60">
+        <f>E60/D60</f>
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <f>H60/F60</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2257,22 +2792,30 @@
         <v>66</v>
       </c>
       <c r="D61">
-        <v>1.616</v>
+        <v>1.6160000000000001</v>
       </c>
       <c r="E61">
-        <v>1.616</v>
+        <v>1.6160000000000001</v>
       </c>
       <c r="F61">
-        <v>-21.79949265599882</v>
+        <v>-21.799492655998819</v>
       </c>
       <c r="G61">
-        <v>-13.48978505940521</v>
+        <v>-13.489785059405211</v>
       </c>
       <c r="H61">
-        <v>-21.79949265599882</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>-21.799492655998819</v>
+      </c>
+      <c r="K61">
+        <f>E61/D61</f>
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <f>H61/F61</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2289,16 +2832,24 @@
         <v>1.502</v>
       </c>
       <c r="F62">
-        <v>-3.214895047684765</v>
+        <v>-3.2148950476847649</v>
       </c>
       <c r="G62">
-        <v>-2.140409485808765</v>
+        <v>-2.1404094858087652</v>
       </c>
       <c r="H62">
-        <v>-3.214895047684765</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>-3.2148950476847649</v>
+      </c>
+      <c r="K62">
+        <f>E62/D62</f>
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <f>H62/F62</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2323,8 +2874,16 @@
       <c r="H63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="K63">
+        <f>E63/D63</f>
+        <v>1</v>
+      </c>
+      <c r="L63" t="e">
+        <f>H63/F63</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2335,10 +2894,10 @@
         <v>69</v>
       </c>
       <c r="D64">
-        <v>1.866</v>
+        <v>1.8660000000000001</v>
       </c>
       <c r="E64">
-        <v>1.866</v>
+        <v>1.8660000000000001</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2349,8 +2908,16 @@
       <c r="H64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="K64">
+        <f>E64/D64</f>
+        <v>1</v>
+      </c>
+      <c r="L64" t="e">
+        <f>H64/F64</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2367,16 +2934,24 @@
         <v>1.006</v>
       </c>
       <c r="F65">
-        <v>7.477381962160287</v>
+        <v>7.4773819621602868</v>
       </c>
       <c r="G65">
         <v>7.432785250656349</v>
       </c>
       <c r="H65">
-        <v>7.477381962160287</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>7.4773819621602868</v>
+      </c>
+      <c r="K65">
+        <f>E65/D65</f>
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <f>H65/F65</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2387,10 +2962,10 @@
         <v>71</v>
       </c>
       <c r="D66">
-        <v>1.689</v>
+        <v>1.6890000000000001</v>
       </c>
       <c r="E66">
-        <v>1.689</v>
+        <v>1.6890000000000001</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -2401,8 +2976,16 @@
       <c r="H66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="K66">
+        <f>E66/D66</f>
+        <v>1</v>
+      </c>
+      <c r="L66" t="e">
+        <f>H66/F66</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2413,10 +2996,10 @@
         <v>72</v>
       </c>
       <c r="D67">
-        <v>3.263</v>
+        <v>3.2629999999999999</v>
       </c>
       <c r="E67">
-        <v>3.263</v>
+        <v>3.2629999999999999</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -2427,8 +3010,16 @@
       <c r="H67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="K67">
+        <f>E67/D67</f>
+        <v>1</v>
+      </c>
+      <c r="L67" t="e">
+        <f>H67/F67</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2439,10 +3030,10 @@
         <v>73</v>
       </c>
       <c r="D68">
-        <v>2.443</v>
+        <v>2.4430000000000001</v>
       </c>
       <c r="E68">
-        <v>2.443</v>
+        <v>2.4430000000000001</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2453,8 +3044,16 @@
       <c r="H68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="K68">
+        <f>E68/D68</f>
+        <v>1</v>
+      </c>
+      <c r="L68" t="e">
+        <f>H68/F68</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2465,10 +3064,10 @@
         <v>74</v>
       </c>
       <c r="D69">
-        <v>1.588</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="E69">
-        <v>1.588</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -2479,8 +3078,16 @@
       <c r="H69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="K69">
+        <f>E69/D69</f>
+        <v>1</v>
+      </c>
+      <c r="L69" t="e">
+        <f>H69/F69</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2491,10 +3098,10 @@
         <v>75</v>
       </c>
       <c r="D70">
-        <v>1.404</v>
+        <v>1.4039999999999999</v>
       </c>
       <c r="E70">
-        <v>1.404</v>
+        <v>1.4039999999999999</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2505,8 +3112,16 @@
       <c r="H70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="K70">
+        <f>E70/D70</f>
+        <v>1</v>
+      </c>
+      <c r="L70" t="e">
+        <f>H70/F70</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2517,22 +3132,30 @@
         <v>76</v>
       </c>
       <c r="D71">
-        <v>1.592086205089574</v>
+        <v>1.5920862050895741</v>
       </c>
       <c r="E71">
-        <v>2.598720578985921</v>
+        <v>2.5987205789859211</v>
       </c>
       <c r="F71">
-        <v>5.064375661482113</v>
+        <v>5.0643756614821127</v>
       </c>
       <c r="G71">
-        <v>3.18096824486786</v>
+        <v>3.1809682448678598</v>
       </c>
       <c r="H71">
-        <v>8.266447639038834</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>8.2664476390388337</v>
+      </c>
+      <c r="K71">
+        <f>E71/D71</f>
+        <v>1.6322737868579871</v>
+      </c>
+      <c r="L71">
+        <f>H71/F71</f>
+        <v>1.6322737868579875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2543,10 +3166,10 @@
         <v>77</v>
       </c>
       <c r="D72">
-        <v>1.467</v>
+        <v>1.4670000000000001</v>
       </c>
       <c r="E72">
-        <v>1.467</v>
+        <v>1.4670000000000001</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -2557,8 +3180,16 @@
       <c r="H72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="K72">
+        <f>E72/D72</f>
+        <v>1</v>
+      </c>
+      <c r="L72" t="e">
+        <f>H72/F72</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2575,16 +3206,24 @@
         <v>2.222</v>
       </c>
       <c r="F73">
-        <v>4.959984944574645</v>
+        <v>4.9599849445746447</v>
       </c>
       <c r="G73">
-        <v>2.23221644670326</v>
+        <v>2.2322164467032599</v>
       </c>
       <c r="H73">
-        <v>4.959984944574645</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>4.9599849445746447</v>
+      </c>
+      <c r="K73">
+        <f>E73/D73</f>
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <f>H73/F73</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2601,16 +3240,24 @@
         <v>1.153</v>
       </c>
       <c r="F74">
-        <v>16.02352614316763</v>
+        <v>16.023526143167629</v>
       </c>
       <c r="G74">
-        <v>13.89724730543593</v>
+        <v>13.897247305435929</v>
       </c>
       <c r="H74">
-        <v>16.02352614316763</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>16.023526143167629</v>
+      </c>
+      <c r="K74">
+        <f>E74/D74</f>
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <f>H74/F74</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2624,19 +3271,27 @@
         <v>1.355</v>
       </c>
       <c r="E75">
-        <v>0.3828303977280408</v>
+        <v>0.38283039772804078</v>
       </c>
       <c r="F75">
         <v>10</v>
       </c>
       <c r="G75">
-        <v>7.380073800738008</v>
+        <v>7.3800738007380078</v>
       </c>
       <c r="H75">
-        <v>2.825316588398825</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>2.8253165883988252</v>
+      </c>
+      <c r="K75">
+        <f>E75/D75</f>
+        <v>0.28253165883988252</v>
+      </c>
+      <c r="L75">
+        <f>H75/F75</f>
+        <v>0.28253165883988252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2650,19 +3305,27 @@
         <v>1.43</v>
       </c>
       <c r="E76">
-        <v>0.4418589499452877</v>
+        <v>0.44185894994528768</v>
       </c>
       <c r="F76">
-        <v>0.2234617293318275</v>
+        <v>0.22346172933182751</v>
       </c>
       <c r="G76">
-        <v>0.1562669435886906</v>
+        <v>0.15626694358869059</v>
       </c>
       <c r="H76">
-        <v>0.06904794760525833</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>6.9047947605258328E-2</v>
+      </c>
+      <c r="K76">
+        <f>E76/D76</f>
+        <v>0.30899227268901236</v>
+      </c>
+      <c r="L76">
+        <f>H76/F76</f>
+        <v>0.30899227268901241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2687,8 +3350,16 @@
       <c r="H77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="K77">
+        <f>E77/D77</f>
+        <v>1</v>
+      </c>
+      <c r="L77" t="e">
+        <f>H77/F77</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2708,13 +3379,21 @@
         <v>-4.541857463865635</v>
       </c>
       <c r="G78">
-        <v>-2.058865577454957</v>
+        <v>-2.0588655774549571</v>
       </c>
       <c r="H78">
         <v>-4.541857463865635</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="K78">
+        <f>E78/D78</f>
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <f>H78/F78</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2725,10 +3404,10 @@
         <v>84</v>
       </c>
       <c r="D79">
-        <v>1.475</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="E79">
-        <v>1.475</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2739,8 +3418,16 @@
       <c r="H79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="K79">
+        <f>E79/D79</f>
+        <v>1</v>
+      </c>
+      <c r="L79" t="e">
+        <f>H79/F79</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2751,10 +3438,10 @@
         <v>85</v>
       </c>
       <c r="D80">
-        <v>4.107</v>
+        <v>4.1070000000000002</v>
       </c>
       <c r="E80">
-        <v>4.107</v>
+        <v>4.1070000000000002</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -2765,8 +3452,16 @@
       <c r="H80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="K80">
+        <f>E80/D80</f>
+        <v>1</v>
+      </c>
+      <c r="L80" t="e">
+        <f>H80/F80</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2777,10 +3472,10 @@
         <v>86</v>
       </c>
       <c r="D81">
-        <v>0.961</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="E81">
-        <v>0.961</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -2791,8 +3486,16 @@
       <c r="H81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="K81">
+        <f>E81/D81</f>
+        <v>1</v>
+      </c>
+      <c r="L81" t="e">
+        <f>H81/F81</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2803,22 +3506,30 @@
         <v>87</v>
       </c>
       <c r="D82">
-        <v>1.199</v>
+        <v>1.1990000000000001</v>
       </c>
       <c r="E82">
-        <v>1.199</v>
+        <v>1.1990000000000001</v>
       </c>
       <c r="F82">
-        <v>4.959984944574645</v>
+        <v>4.9599849445746447</v>
       </c>
       <c r="G82">
-        <v>4.136768093890446</v>
+        <v>4.1367680938904456</v>
       </c>
       <c r="H82">
-        <v>4.959984944574645</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>4.9599849445746447</v>
+      </c>
+      <c r="K82">
+        <f>E82/D82</f>
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <f>H82/F82</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2838,13 +3549,21 @@
         <v>-29.1758271355658</v>
       </c>
       <c r="G83">
-        <v>-24.39450429395134</v>
+        <v>-24.394504293951339</v>
       </c>
       <c r="H83">
         <v>-29.1758271355658</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="K83">
+        <f>E83/D83</f>
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <f>H83/F83</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2855,22 +3574,30 @@
         <v>89</v>
       </c>
       <c r="D84">
-        <v>1.291</v>
+        <v>1.2909999999999999</v>
       </c>
       <c r="E84">
-        <v>0.3361840385267708</v>
+        <v>0.33618403852677081</v>
       </c>
       <c r="F84">
-        <v>6.007249575350357</v>
+        <v>6.0072495753503574</v>
       </c>
       <c r="G84">
-        <v>4.653175503757055</v>
+        <v>4.6531755037570548</v>
       </c>
       <c r="H84">
         <v>1.564323332826888</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="K84">
+        <f>E84/D84</f>
+        <v>0.26040591675195263</v>
+      </c>
+      <c r="L84">
+        <f>H84/F84</f>
+        <v>0.26040591675195263</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2895,8 +3622,16 @@
       <c r="H85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="K85">
+        <f>E85/D85</f>
+        <v>1</v>
+      </c>
+      <c r="L85" t="e">
+        <f>H85/F85</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2907,10 +3642,10 @@
         <v>91</v>
       </c>
       <c r="D86">
-        <v>1.352</v>
+        <v>1.3520000000000001</v>
       </c>
       <c r="E86">
-        <v>1.352</v>
+        <v>1.3520000000000001</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -2921,8 +3656,16 @@
       <c r="H86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="K86">
+        <f>E86/D86</f>
+        <v>1</v>
+      </c>
+      <c r="L86" t="e">
+        <f>H86/F86</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2936,7 +3679,7 @@
         <v>1.738</v>
       </c>
       <c r="E87">
-        <v>0.7331540333790081</v>
+        <v>0.73315403337900809</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -2947,8 +3690,16 @@
       <c r="H87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="K87">
+        <f>E87/D87</f>
+        <v>0.42183776373936022</v>
+      </c>
+      <c r="L87" t="e">
+        <f>H87/F87</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2959,10 +3710,10 @@
         <v>93</v>
       </c>
       <c r="D88">
-        <v>3.054</v>
+        <v>3.0539999999999998</v>
       </c>
       <c r="E88">
-        <v>2.719186640164933</v>
+        <v>2.7191866401649332</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -2973,8 +3724,16 @@
       <c r="H88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="K88">
+        <f>E88/D88</f>
+        <v>0.89036890640633048</v>
+      </c>
+      <c r="L88" t="e">
+        <f>H88/F88</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2985,22 +3744,30 @@
         <v>94</v>
       </c>
       <c r="D89">
-        <v>0.823</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="E89">
-        <v>0.09641442113039941</v>
+        <v>9.6414421130399414E-2</v>
       </c>
       <c r="F89">
-        <v>5.064375661482113</v>
+        <v>5.0643756614821127</v>
       </c>
       <c r="G89">
-        <v>6.153554874218849</v>
+        <v>6.1535548742188491</v>
       </c>
       <c r="H89">
-        <v>0.5932914310919581</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>0.59329143109195814</v>
+      </c>
+      <c r="K89">
+        <f>E89/D89</f>
+        <v>0.11714996492150598</v>
+      </c>
+      <c r="L89">
+        <f>H89/F89</f>
+        <v>0.11714996492150598</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3011,10 +3778,10 @@
         <v>95</v>
       </c>
       <c r="D90">
-        <v>1.535</v>
+        <v>1.5349999999999999</v>
       </c>
       <c r="E90">
-        <v>1.535</v>
+        <v>1.5349999999999999</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3025,8 +3792,16 @@
       <c r="H90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="K90">
+        <f>E90/D90</f>
+        <v>1</v>
+      </c>
+      <c r="L90" t="e">
+        <f>H90/F90</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3051,8 +3826,16 @@
       <c r="H91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="K91">
+        <f>E91/D91</f>
+        <v>1</v>
+      </c>
+      <c r="L91" t="e">
+        <f>H91/F91</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3063,22 +3846,30 @@
         <v>97</v>
       </c>
       <c r="D92">
-        <v>2.123</v>
+        <v>2.1230000000000002</v>
       </c>
       <c r="E92">
-        <v>1.201979012270128</v>
+        <v>1.2019790122701279</v>
       </c>
       <c r="F92">
-        <v>38.53460965051551</v>
+        <v>38.534609650515513</v>
       </c>
       <c r="G92">
-        <v>18.15101726354946</v>
+        <v>18.151017263549459</v>
       </c>
       <c r="H92">
-        <v>21.81714180213921</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>21.817141802139211</v>
+      </c>
+      <c r="K92">
+        <f>E92/D92</f>
+        <v>0.56617004817245775</v>
+      </c>
+      <c r="L92">
+        <f>H92/F92</f>
+        <v>0.56617004817245742</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3103,8 +3894,16 @@
       <c r="H93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="K93">
+        <f>E93/D93</f>
+        <v>1</v>
+      </c>
+      <c r="L93" t="e">
+        <f>H93/F93</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3121,16 +3920,24 @@
         <v>1.022</v>
       </c>
       <c r="F94">
-        <v>4.765319193197463</v>
+        <v>4.7653191931974632</v>
       </c>
       <c r="G94">
-        <v>4.662738936592429</v>
+        <v>4.6627389365924294</v>
       </c>
       <c r="H94">
-        <v>4.765319193197463</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>4.7653191931974632</v>
+      </c>
+      <c r="K94">
+        <f>E94/D94</f>
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <f>H94/F94</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3147,16 +3954,24 @@
         <v>1.37</v>
       </c>
       <c r="F95">
-        <v>21.79949265599882</v>
+        <v>21.799492655998819</v>
       </c>
       <c r="G95">
         <v>15.91203843503563</v>
       </c>
       <c r="H95">
-        <v>21.79949265599882</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>21.799492655998819</v>
+      </c>
+      <c r="K95">
+        <f>E95/D95</f>
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <f>H95/F95</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3167,22 +3982,30 @@
         <v>101</v>
       </c>
       <c r="D96">
-        <v>1.435</v>
+        <v>1.4350000000000001</v>
       </c>
       <c r="E96">
-        <v>0.4459615921542046</v>
+        <v>0.44596159215420461</v>
       </c>
       <c r="F96">
-        <v>9.282532599166634</v>
+        <v>9.2825325991666343</v>
       </c>
       <c r="G96">
-        <v>6.46866383217187</v>
+        <v>6.4686638321718704</v>
       </c>
       <c r="H96">
         <v>2.884775621705685</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="K96">
+        <f>E96/D96</f>
+        <v>0.31077462867888822</v>
+      </c>
+      <c r="L96">
+        <f>H96/F96</f>
+        <v>0.31077462867888811</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3205,10 +4028,18 @@
         <v>5.882352941176471</v>
       </c>
       <c r="H97">
-        <v>20.11176470588235</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>20.111764705882351</v>
+      </c>
+      <c r="K97">
+        <f>E97/D97</f>
+        <v>2.0111764705882353</v>
+      </c>
+      <c r="L97">
+        <f>H97/F97</f>
+        <v>2.0111764705882349</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3231,7 +4062,15 @@
         <v>5.882352941176471</v>
       </c>
       <c r="H98">
-        <v>20.11176470588235</v>
+        <v>20.111764705882351</v>
+      </c>
+      <c r="K98">
+        <f>E98/D98</f>
+        <v>2.0111764705882353</v>
+      </c>
+      <c r="L98">
+        <f>H98/F98</f>
+        <v>2.0111764705882349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>